<commit_message>
add update to script to do pts filter
</commit_message>
<xml_diff>
--- a/src/top_genes_cluster_0.4.xlsx
+++ b/src/top_genes_cluster_0.4.xlsx
@@ -538,39 +538,39 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Ptprb</t>
+          <t>Clec14a</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>24.30417060852051</v>
+        <v>9.153927803039551</v>
       </c>
       <c r="C5" t="n">
-        <v>4.537421226501465</v>
+        <v>4.631550312042236</v>
       </c>
       <c r="D5" t="n">
-        <v>9.254136655594219e-127</v>
+        <v>5.680524071573974e-18</v>
       </c>
       <c r="E5" t="n">
-        <v>0.942652329749104</v>
+        <v>0.3476702508960574</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Mecom</t>
+          <t>Ptprb</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>24.45771980285645</v>
+        <v>24.30417060852051</v>
       </c>
       <c r="C6" t="n">
-        <v>4.508071422576904</v>
+        <v>4.537421226501465</v>
       </c>
       <c r="D6" t="n">
-        <v>2.90203174931901e-128</v>
+        <v>9.254136655594219e-127</v>
       </c>
       <c r="E6" t="n">
-        <v>0.974910394265233</v>
+        <v>0.942652329749104</v>
       </c>
     </row>
   </sheetData>
@@ -772,77 +772,77 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Ranbp3l</t>
+          <t>Igfbp3</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12.89632034301758</v>
+        <v>5.603856086730957</v>
       </c>
       <c r="C3" t="n">
-        <v>2.10603666305542</v>
+        <v>2.349907636642456</v>
       </c>
       <c r="D3" t="n">
-        <v>2.466879160583189e-34</v>
+        <v>3.71320565257575e-06</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8926829268292683</v>
+        <v>0.3024390243902439</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Slc7a11</t>
+          <t>Pla1a</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>13.03956604003906</v>
+        <v>6.086055755615234</v>
       </c>
       <c r="C4" t="n">
-        <v>2.0783531665802</v>
+        <v>2.349749326705933</v>
       </c>
       <c r="D4" t="n">
-        <v>7.425888279816912e-35</v>
+        <v>2.573184392021096e-07</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8634146341463415</v>
+        <v>0.3121951219512195</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Medag</t>
+          <t>Ranbp3l</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7.80372428894043</v>
+        <v>12.89632034301758</v>
       </c>
       <c r="C5" t="n">
-        <v>2.009799003601074</v>
+        <v>2.10603666305542</v>
       </c>
       <c r="D5" t="n">
-        <v>2.85519262621867e-12</v>
+        <v>2.466879160583189e-34</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4536585365853659</v>
+        <v>0.8926829268292683</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Aldh1a2</t>
+          <t>Slc7a11</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>9.759799003601074</v>
+        <v>13.03956604003906</v>
       </c>
       <c r="C6" t="n">
-        <v>1.90752899646759</v>
+        <v>2.0783531665802</v>
       </c>
       <c r="D6" t="n">
-        <v>1.522019734757183e-19</v>
+        <v>7.425888279816912e-35</v>
       </c>
       <c r="E6" t="n">
-        <v>0.624390243902439</v>
+        <v>0.8634146341463415</v>
       </c>
     </row>
   </sheetData>
@@ -889,96 +889,96 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Rpl18a</t>
+          <t>Ftl1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8.461723327636719</v>
+        <v>7.98644495010376</v>
       </c>
       <c r="C2" t="n">
-        <v>3.634722232818604</v>
+        <v>3.640774965286255</v>
       </c>
       <c r="D2" t="n">
-        <v>2.202588431015998e-14</v>
+        <v>7.257124971693554e-13</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4019607843137255</v>
+        <v>0.3823529411764706</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Rpl41</t>
+          <t>Rpl18a</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10.50026988983154</v>
+        <v>8.461723327636719</v>
       </c>
       <c r="C3" t="n">
-        <v>3.580030679702759</v>
+        <v>3.634722232818604</v>
       </c>
       <c r="D3" t="n">
-        <v>1.800275661234721e-22</v>
+        <v>2.202588431015998e-14</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5098039215686274</v>
+        <v>0.4019607843137255</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Rps23</t>
+          <t>Rpl19</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8.355746269226074</v>
+        <v>7.77732515335083</v>
       </c>
       <c r="C4" t="n">
-        <v>3.565969705581665</v>
+        <v>3.607499599456787</v>
       </c>
       <c r="D4" t="n">
-        <v>4.686185945897644e-14</v>
+        <v>3.365697566386239e-12</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4019607843137255</v>
+        <v>0.3725490196078431</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Rplp1</t>
+          <t>Rpl41</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.17930316925049</v>
+        <v>10.50026988983154</v>
       </c>
       <c r="C5" t="n">
-        <v>3.563366651535034</v>
+        <v>3.580030679702759</v>
       </c>
       <c r="D5" t="n">
-        <v>2.093705484313558e-30</v>
+        <v>1.800275661234721e-22</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.5098039215686274</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Fau</t>
+          <t>Rps23</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>8.611340522766113</v>
+        <v>8.355746269226074</v>
       </c>
       <c r="C6" t="n">
-        <v>3.546496152877808</v>
+        <v>3.565969705581665</v>
       </c>
       <c r="D6" t="n">
-        <v>6.562109393644657e-15</v>
+        <v>4.686185945897644e-14</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.4019607843137255</v>
       </c>
     </row>
   </sheetData>
@@ -1063,58 +1063,58 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Lama1</t>
+          <t>Grem2</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8.608819961547852</v>
+        <v>7.478861331939697</v>
       </c>
       <c r="C4" t="n">
-        <v>2.092109441757202</v>
+        <v>2.485360860824585</v>
       </c>
       <c r="D4" t="n">
-        <v>5.277788182782912e-15</v>
+        <v>3.482079853079695e-11</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Col4a6</t>
+          <t>Aox3</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.52660942077637</v>
+        <v>7.725160121917725</v>
       </c>
       <c r="C5" t="n">
-        <v>2.079169988632202</v>
+        <v>2.30659556388855</v>
       </c>
       <c r="D5" t="n">
-        <v>1.04727916447729e-22</v>
+        <v>5.559300436662962e-12</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5357142857142857</v>
+        <v>0.3714285714285714</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Ltbp1</t>
+          <t>Tmem132c</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>11.33651924133301</v>
+        <v>6.671573162078857</v>
       </c>
       <c r="C6" t="n">
-        <v>2.029100179672241</v>
+        <v>2.137815475463867</v>
       </c>
       <c r="D6" t="n">
-        <v>2.260390717954911e-26</v>
+        <v>8.396090083369488e-09</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5964285714285714</v>
+        <v>0.3357142857142857</v>
       </c>
     </row>
   </sheetData>
@@ -1161,96 +1161,96 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Igf1</t>
+          <t>Tmem132e</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17.9183349609375</v>
+        <v>7.111780166625977</v>
       </c>
       <c r="C2" t="n">
-        <v>3.092049598693848</v>
+        <v>3.38364577293396</v>
       </c>
       <c r="D2" t="n">
-        <v>8.865119719549452e-68</v>
+        <v>1.961631211988044e-10</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9393939393939394</v>
+        <v>0.3383838383838384</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Ltbp1</t>
+          <t>Igf1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>16.49800491333008</v>
+        <v>17.9183349609375</v>
       </c>
       <c r="C3" t="n">
-        <v>3.040301084518433</v>
+        <v>3.092049598693848</v>
       </c>
       <c r="D3" t="n">
-        <v>1.981494228641063e-57</v>
+        <v>8.865119719549452e-68</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8484848484848485</v>
+        <v>0.9393939393939394</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Grem2</t>
+          <t>Ltbp1</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10.15969562530518</v>
+        <v>16.49800491333008</v>
       </c>
       <c r="C4" t="n">
-        <v>2.973413467407227</v>
+        <v>3.040301084518433</v>
       </c>
       <c r="D4" t="n">
-        <v>1.306358055235668e-21</v>
+        <v>1.981494228641063e-57</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5101010101010101</v>
+        <v>0.8484848484848485</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Svep1</t>
+          <t>Grem2</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>13.78193855285645</v>
+        <v>10.15969562530518</v>
       </c>
       <c r="C5" t="n">
-        <v>2.91600775718689</v>
+        <v>2.973413467407227</v>
       </c>
       <c r="D5" t="n">
-        <v>5.263196384214766e-40</v>
+        <v>1.306358055235668e-21</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7121212121212122</v>
+        <v>0.5101010101010101</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Igfbp2</t>
+          <t>Svep1</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>13.24851512908936</v>
+        <v>13.78193855285645</v>
       </c>
       <c r="C6" t="n">
-        <v>2.875304937362671</v>
+        <v>2.91600775718689</v>
       </c>
       <c r="D6" t="n">
-        <v>6.412683480906885e-37</v>
+        <v>5.263196384214766e-40</v>
       </c>
       <c r="E6" t="n">
-        <v>0.696969696969697</v>
+        <v>0.7121212121212122</v>
       </c>
     </row>
   </sheetData>
@@ -1373,20 +1373,20 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Col13a1</t>
+          <t>Tbx18</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5.686466217041016</v>
+        <v>5.165728092193604</v>
       </c>
       <c r="C6" t="n">
-        <v>3.199073314666748</v>
+        <v>4.254248142242432</v>
       </c>
       <c r="D6" t="n">
-        <v>4.928649590142774e-06</v>
+        <v>6.764717505333729e-05</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4111111111111111</v>
+        <v>0.3444444444444444</v>
       </c>
     </row>
   </sheetData>
@@ -1607,58 +1607,58 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Notch3</t>
+          <t>Gm12002</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>19.91693878173828</v>
+        <v>7.802682399749756</v>
       </c>
       <c r="C4" t="n">
-        <v>5.95043420791626</v>
+        <v>6.187079429626465</v>
       </c>
       <c r="D4" t="n">
-        <v>1.010888609432314e-84</v>
+        <v>8.279112683654652e-13</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8783068783068783</v>
+        <v>0.3439153439153439</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Tbx3os1</t>
+          <t>Notch3</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>15.91995525360107</v>
+        <v>19.91693878173828</v>
       </c>
       <c r="C5" t="n">
-        <v>5.90712833404541</v>
+        <v>5.95043420791626</v>
       </c>
       <c r="D5" t="n">
-        <v>4.376945966447012e-54</v>
+        <v>1.010888609432314e-84</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7037037037037037</v>
+        <v>0.8783068783068783</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Trpc3</t>
+          <t>Tbx3os1</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>18.31001472473145</v>
+        <v>15.91995525360107</v>
       </c>
       <c r="C6" t="n">
-        <v>5.889199256896973</v>
+        <v>5.90712833404541</v>
       </c>
       <c r="D6" t="n">
-        <v>1.308246644135486e-71</v>
+        <v>4.376945966447012e-54</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8095238095238095</v>
+        <v>0.7037037037037037</v>
       </c>
     </row>
   </sheetData>
@@ -1705,96 +1705,96 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Slc47a1</t>
+          <t>Myoc</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16.18927574157715</v>
+        <v>5.7233567237854</v>
       </c>
       <c r="C2" t="n">
-        <v>4.450317859649658</v>
+        <v>5.037930011749268</v>
       </c>
       <c r="D2" t="n">
-        <v>1.254710437143614e-54</v>
+        <v>1.254535432636743e-06</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9910714285714286</v>
+        <v>0.3303571428571428</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Tbx15</t>
+          <t>Gm973</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10.17861366271973</v>
+        <v>6.428671360015869</v>
       </c>
       <c r="C3" t="n">
-        <v>4.307960510253906</v>
+        <v>4.575037956237793</v>
       </c>
       <c r="D3" t="n">
-        <v>1.475351188655028e-21</v>
+        <v>2.118475017243618e-08</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6071428571428571</v>
+        <v>0.3839285714285715</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Tspan11</t>
+          <t>Prps2</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>14.02823543548584</v>
+        <v>6.665574550628662</v>
       </c>
       <c r="C4" t="n">
-        <v>4.153435230255127</v>
+        <v>4.530786037445068</v>
       </c>
       <c r="D4" t="n">
-        <v>2.736063121309078e-41</v>
+        <v>4.669635598598761e-09</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8482142857142857</v>
+        <v>0.3928571428571428</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Slc4a10</t>
+          <t>Slc47a1</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>15.75197792053223</v>
+        <v>16.18927574157715</v>
       </c>
       <c r="C5" t="n">
-        <v>4.049439907073975</v>
+        <v>4.450317859649658</v>
       </c>
       <c r="D5" t="n">
-        <v>6.956507806217545e-52</v>
+        <v>1.254710437143614e-54</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>0.9910714285714286</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Slc47a2</t>
+          <t>Tbx15</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>11.57633876800537</v>
+        <v>10.17861366271973</v>
       </c>
       <c r="C6" t="n">
-        <v>3.94968843460083</v>
+        <v>4.307960510253906</v>
       </c>
       <c r="D6" t="n">
-        <v>6.307103822333806e-28</v>
+        <v>1.475351188655028e-21</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7053571428571429</v>
+        <v>0.6071428571428571</v>
       </c>
     </row>
   </sheetData>
@@ -1841,96 +1841,96 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Bmx</t>
+          <t>Sema3g</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10.23504638671875</v>
+        <v>5.77971363067627</v>
       </c>
       <c r="C2" t="n">
-        <v>6.608002662658691</v>
+        <v>7.014009952545166</v>
       </c>
       <c r="D2" t="n">
-        <v>2.062170293983623e-21</v>
+        <v>1.109204878479648e-06</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6477272727272727</v>
+        <v>0.3636363636363636</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Prdm16</t>
+          <t>Bmx</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10.99948310852051</v>
+        <v>10.23504638671875</v>
       </c>
       <c r="C3" t="n">
-        <v>5.73930025100708</v>
+        <v>6.608002662658691</v>
       </c>
       <c r="D3" t="n">
-        <v>8.925358263575392e-25</v>
+        <v>2.062170293983623e-21</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7045454545454546</v>
+        <v>0.6477272727272727</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Lama3</t>
+          <t>Nos1</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7.815247058868408</v>
+        <v>5.670414447784424</v>
       </c>
       <c r="C4" t="n">
-        <v>4.904033184051514</v>
+        <v>5.827220439910889</v>
       </c>
       <c r="D4" t="n">
-        <v>2.204871793142434e-12</v>
+        <v>2.011758290660017e-06</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5113636363636364</v>
+        <v>0.3636363636363636</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Vegfc</t>
+          <t>Prdm16</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.94721031188965</v>
+        <v>10.99948310852051</v>
       </c>
       <c r="C5" t="n">
-        <v>4.55402660369873</v>
+        <v>5.73930025100708</v>
       </c>
       <c r="D5" t="n">
-        <v>1.432260703817273e-24</v>
+        <v>8.925358263575392e-25</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7272727272727273</v>
+        <v>0.7045454545454546</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Plcg2</t>
+          <t>Lama3</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7.238114833831787</v>
+        <v>7.815247058868408</v>
       </c>
       <c r="C6" t="n">
-        <v>4.15699291229248</v>
+        <v>4.904033184051514</v>
       </c>
       <c r="D6" t="n">
-        <v>1.440790354687923e-10</v>
+        <v>2.204871793142434e-12</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4886363636363636</v>
+        <v>0.5113636363636364</v>
       </c>
     </row>
   </sheetData>
@@ -2053,20 +2053,20 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Slc6a20a</t>
+          <t>Ppp1r1a</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>14.18364715576172</v>
+        <v>5.995941162109375</v>
       </c>
       <c r="C6" t="n">
-        <v>2.439021587371826</v>
+        <v>2.513557195663452</v>
       </c>
       <c r="D6" t="n">
-        <v>6.044269318625661e-42</v>
+        <v>7.550876496636515e-07</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8920454545454546</v>
+        <v>0.3409090909090909</v>
       </c>
     </row>
   </sheetData>
@@ -2268,77 +2268,77 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Nox4</t>
+          <t>Angptl1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7.003499031066895</v>
+        <v>4.304681777954102</v>
       </c>
       <c r="C3" t="n">
-        <v>4.927291393280029</v>
+        <v>5.369338035583496</v>
       </c>
       <c r="D3" t="n">
-        <v>3.06934761341701e-09</v>
+        <v>0.002859872853422683</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5925925925925926</v>
+        <v>0.3518518518518519</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Col14a1</t>
+          <t>Nox4</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5.971248626708984</v>
+        <v>7.003499031066895</v>
       </c>
       <c r="C4" t="n">
-        <v>4.874123096466064</v>
+        <v>4.927291393280029</v>
       </c>
       <c r="D4" t="n">
-        <v>1.366950806119628e-06</v>
+        <v>3.06934761341701e-09</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5</v>
+        <v>0.5925925925925926</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Rspo2</t>
+          <t>Col14a1</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5.993216991424561</v>
+        <v>5.971248626708984</v>
       </c>
       <c r="C5" t="n">
-        <v>4.676848888397217</v>
+        <v>4.874123096466064</v>
       </c>
       <c r="D5" t="n">
-        <v>1.264694910126828e-06</v>
+        <v>1.366950806119628e-06</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5185185185185185</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Fndc1</t>
+          <t>Gfpt2</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>8.145654678344727</v>
+        <v>3.939765214920044</v>
       </c>
       <c r="C6" t="n">
-        <v>4.639036655426025</v>
+        <v>4.800660610198975</v>
       </c>
       <c r="D6" t="n">
-        <v>1.314102389259921e-12</v>
+        <v>0.01065446690907652</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6851851851851852</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -2948,77 +2948,77 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Adgrl4</t>
+          <t>Slco1c1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6.849327564239502</v>
+        <v>4.474020481109619</v>
       </c>
       <c r="C3" t="n">
-        <v>2.203131437301636</v>
+        <v>2.42079496383667</v>
       </c>
       <c r="D3" t="n">
-        <v>2.349714339750008e-09</v>
+        <v>0.0005093369476376944</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5304347826086957</v>
+        <v>0.3217391304347826</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Tmtc2</t>
+          <t>Spock2</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8.723294258117676</v>
+        <v>3.735859632492065</v>
       </c>
       <c r="C4" t="n">
-        <v>2.179532766342163</v>
+        <v>2.281996488571167</v>
       </c>
       <c r="D4" t="n">
-        <v>2.97259115242356e-15</v>
+        <v>0.007636826084559388</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7217391304347827</v>
+        <v>0.3130434782608696</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Lef1</t>
+          <t>Adgrl4</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5.322223663330078</v>
+        <v>6.849327564239502</v>
       </c>
       <c r="C5" t="n">
-        <v>1.79841685295105</v>
+        <v>2.203131437301636</v>
       </c>
       <c r="D5" t="n">
-        <v>1.245630520566503e-05</v>
+        <v>2.349714339750008e-09</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4608695652173913</v>
+        <v>0.5304347826086957</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Mecom</t>
+          <t>Tmtc2</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6.548807621002197</v>
+        <v>8.723294258117676</v>
       </c>
       <c r="C6" t="n">
-        <v>1.718349933624268</v>
+        <v>2.179532766342163</v>
       </c>
       <c r="D6" t="n">
-        <v>1.478321622020316e-08</v>
+        <v>2.97259115242356e-15</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6173913043478261</v>
+        <v>0.7217391304347827</v>
       </c>
     </row>
   </sheetData>
@@ -3084,77 +3084,77 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gria3</t>
+          <t>Cntnap5b</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.638855218887329</v>
+        <v>3.528460264205933</v>
       </c>
       <c r="C3" t="n">
-        <v>1.027507901191711</v>
+        <v>1.252711772918701</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01621328852190851</v>
+        <v>0.02151797131806221</v>
       </c>
       <c r="E3" t="n">
-        <v>0.412</v>
+        <v>0.356</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Kirrel3</t>
+          <t>Gria3</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.181618690490723</v>
+        <v>3.638855218887329</v>
       </c>
       <c r="C4" t="n">
-        <v>1.027142882347107</v>
+        <v>1.027507901191711</v>
       </c>
       <c r="D4" t="n">
-        <v>3.489781664528542e-07</v>
+        <v>0.01621328852190851</v>
       </c>
       <c r="E4" t="n">
-        <v>0.616</v>
+        <v>0.412</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Lsamp</t>
+          <t>Kirrel3</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.45835208892822</v>
+        <v>6.181618690490723</v>
       </c>
       <c r="C5" t="n">
-        <v>1.014389038085938</v>
+        <v>1.027142882347107</v>
       </c>
       <c r="D5" t="n">
-        <v>2.80427248342351e-21</v>
+        <v>3.489781664528542e-07</v>
       </c>
       <c r="E5" t="n">
-        <v>0.948</v>
+        <v>0.616</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Kcnip4</t>
+          <t>Lsamp</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>9.061214447021484</v>
+        <v>10.45835208892822</v>
       </c>
       <c r="C6" t="n">
-        <v>1.01419723033905</v>
+        <v>1.014389038085938</v>
       </c>
       <c r="D6" t="n">
-        <v>8.987870401271418e-16</v>
+        <v>2.80427248342351e-21</v>
       </c>
       <c r="E6" t="n">
-        <v>0.872</v>
+        <v>0.948</v>
       </c>
     </row>
   </sheetData>
@@ -3666,39 +3666,39 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Nostrin</t>
+          <t>Tfrc</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>9.850622177124023</v>
+        <v>8.758108139038086</v>
       </c>
       <c r="C5" t="n">
-        <v>3.98274040222168</v>
+        <v>3.983325242996216</v>
       </c>
       <c r="D5" t="n">
-        <v>1.095224244319312e-20</v>
+        <v>2.545998775480264e-16</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4105691056910569</v>
+        <v>0.3699186991869919</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Prom1</t>
+          <t>Nostrin</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>10.39366340637207</v>
+        <v>9.850622177124023</v>
       </c>
       <c r="C6" t="n">
-        <v>3.937930822372437</v>
+        <v>3.98274040222168</v>
       </c>
       <c r="D6" t="n">
-        <v>4.815862846041939e-23</v>
+        <v>1.095224244319312e-20</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4308943089430894</v>
+        <v>0.4105691056910569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>